<commit_message>
adding answers from wildcard
</commit_message>
<xml_diff>
--- a/2019MEP/MMM19_AAnswers_templ.xlsx
+++ b/2019MEP/MMM19_AAnswers_templ.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="76">
   <si>
     <t xml:space="preserve">Wildcard </t>
   </si>
@@ -1070,12 +1070,15 @@
       <c r="D20" s="4"/>
       <c r="L20" s="4"/>
       <c r="M20" s="1"/>
-      <c r="N20" s="14">
+      <c r="N20" s="14" t="str">
         <f>P20</f>
-        <v>0</v>
+        <v>Antlion</v>
       </c>
       <c r="O20">
         <v>16</v>
+      </c>
+      <c r="P20" t="s">
+        <v>70</v>
       </c>
       <c r="Q20" s="11" t="s">
         <v>71</v>

</xml_diff>